<commit_message>
pok upload final 1
</commit_message>
<xml_diff>
--- a/uploaded/pok/a.xlsx
+++ b/uploaded/pok/a.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RKAKLDIPA17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\_muh.shamad\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="POKREV5" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -2126,8 +2126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G546"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2138,6 +2138,7 @@
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>